<commit_message>
Adicionando passos no roteiro
</commit_message>
<xml_diff>
--- a/TerceiroPasso/DetalhesReserva.xlsx
+++ b/TerceiroPasso/DetalhesReserva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTI DIGITAL\Desktop\DTI Digital\roteirosDeTeste\TerceiroPasso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D2E752A-1FE9-4812-B43F-CA71996891A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB0ED259-0F01-460D-871D-EBBE6D75E08C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
   <si>
     <t>CHECKLIST FLOW</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Deve aparecer o nome do grupo selecionado para reserva</t>
+  </si>
+  <si>
+    <t>Componente fixo</t>
+  </si>
+  <si>
+    <t>O Componente deve ser fixo na tela e acompanhar toda a rolagem, mas ao chegar no rodapé ele deve parar de acompanhar a página</t>
+  </si>
+  <si>
+    <t>Dados NR</t>
+  </si>
+  <si>
+    <t>Os dados para preencher o componente devem ser pegos da Store</t>
   </si>
   <si>
     <t>CHECKLIST DEVELOPER</t>
@@ -1046,11 +1058,11 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1081,16 +1093,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1101,6 +1107,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7502,8 +7514,8 @@
   </sheetPr>
   <dimension ref="A2:AMK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -7656,10 +7668,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="62"/>
+      <c r="B11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15" t="s">
         <v>24</v>
@@ -7668,10 +7684,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="62"/>
+      <c r="B12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="14"/>
       <c r="E12" s="15" t="s">
         <v>24</v>
@@ -8201,26 +8221,26 @@
     <row r="1" spans="2:4" s="1" customFormat="1"/>
     <row r="2" spans="2:4" ht="18" customHeight="1">
       <c r="B2" s="63" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
     </row>
     <row r="3" spans="2:4" ht="13.9" customHeight="1">
       <c r="B3" s="70" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="70"/>
       <c r="C4" s="17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>24</v>
@@ -8233,10 +8253,10 @@
     </row>
     <row r="6" spans="2:4" ht="13.9" customHeight="1">
       <c r="B6" s="70" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>24</v>
@@ -8245,7 +8265,7 @@
     <row r="7" spans="2:4" ht="25.5">
       <c r="B7" s="70"/>
       <c r="C7" s="19" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>24</v>
@@ -8254,7 +8274,7 @@
     <row r="8" spans="2:4">
       <c r="B8" s="70"/>
       <c r="C8" s="19" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>24</v>
@@ -8263,7 +8283,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="70"/>
       <c r="C9" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>24</v>
@@ -8272,7 +8292,7 @@
     <row r="10" spans="2:4">
       <c r="B10" s="70"/>
       <c r="C10" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>24</v>
@@ -8281,7 +8301,7 @@
     <row r="11" spans="2:4">
       <c r="B11" s="70"/>
       <c r="C11" s="19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>24</v>
@@ -8294,10 +8314,10 @@
     </row>
     <row r="13" spans="2:4" ht="23.85" customHeight="1">
       <c r="B13" s="68" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>24</v>
@@ -8306,7 +8326,7 @@
     <row r="14" spans="2:4" ht="25.5">
       <c r="B14" s="68"/>
       <c r="C14" s="19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>24</v>
@@ -8315,7 +8335,7 @@
     <row r="15" spans="2:4" ht="25.5">
       <c r="B15" s="68"/>
       <c r="C15" s="19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>24</v>
@@ -8324,7 +8344,7 @@
     <row r="16" spans="2:4">
       <c r="B16" s="68"/>
       <c r="C16" s="17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>24</v>
@@ -8333,7 +8353,7 @@
     <row r="17" spans="2:4">
       <c r="B17" s="68"/>
       <c r="C17" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>24</v>
@@ -8342,7 +8362,7 @@
     <row r="18" spans="2:4">
       <c r="B18" s="68"/>
       <c r="C18" s="17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>24</v>
@@ -8351,7 +8371,7 @@
     <row r="19" spans="2:4">
       <c r="B19" s="68"/>
       <c r="C19" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>24</v>
@@ -8360,7 +8380,7 @@
     <row r="20" spans="2:4" ht="25.5">
       <c r="B20" s="68"/>
       <c r="C20" s="19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>24</v>
@@ -8373,10 +8393,10 @@
     </row>
     <row r="22" spans="2:4" ht="13.9" customHeight="1">
       <c r="B22" s="68" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>24</v>
@@ -8385,7 +8405,7 @@
     <row r="23" spans="2:4" ht="25.5">
       <c r="B23" s="68"/>
       <c r="C23" s="19" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>24</v>
@@ -8394,7 +8414,7 @@
     <row r="24" spans="2:4" ht="17.45" customHeight="1">
       <c r="B24" s="68"/>
       <c r="C24" s="19" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>24</v>
@@ -8407,10 +8427,10 @@
     </row>
     <row r="26" spans="2:4" ht="13.9" customHeight="1">
       <c r="B26" s="68" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>24</v>
@@ -8419,7 +8439,7 @@
     <row r="27" spans="2:4" ht="25.5">
       <c r="B27" s="68"/>
       <c r="C27" s="19" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>24</v>
@@ -8428,7 +8448,7 @@
     <row r="28" spans="2:4">
       <c r="B28" s="68"/>
       <c r="C28" s="19" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>24</v>
@@ -8440,11 +8460,11 @@
     <row r="32" spans="2:4" s="1" customFormat="1"/>
     <row r="33" spans="2:4" s="1" customFormat="1" ht="17.45" customHeight="1">
       <c r="B33" s="69" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C33" s="69"/>
       <c r="D33" s="21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:4" s="1" customFormat="1"/>
@@ -8673,61 +8693,61 @@
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="18">
-      <c r="B2" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="B2" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="B3" s="72" t="s">
-        <v>72</v>
+      <c r="B3" s="73" t="s">
+        <v>76</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="B4" s="72"/>
+      <c r="B4" s="73"/>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="B5" s="72"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="27" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="B6" s="72"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="77" t="s">
-        <v>77</v>
+      <c r="B8" s="75" t="s">
+        <v>81</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>24</v>
@@ -8735,45 +8755,45 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="77"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="27" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="B10" s="77"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="27" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="B11" s="77"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="B12" s="77"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="27" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="B13" s="77"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>24</v>
@@ -8781,9 +8801,9 @@
     </row>
     <row r="14" spans="1:19" s="29" customFormat="1">
       <c r="A14" s="28"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -8801,11 +8821,11 @@
       <c r="S14" s="28"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="B15" s="72" t="s">
-        <v>84</v>
+      <c r="B15" s="73" t="s">
+        <v>88</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>24</v>
@@ -8813,34 +8833,34 @@
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="B16" s="72"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="73" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="72"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>24</v>
@@ -8853,29 +8873,29 @@
       <c r="D20" s="34"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="72" t="s">
-        <v>89</v>
+      <c r="B21" s="73" t="s">
+        <v>93</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="72"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="35" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="72"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="35" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>24</v>
@@ -8897,12 +8917,12 @@
       <c r="D26" s="38"/>
     </row>
     <row r="27" spans="2:5" ht="18.75">
-      <c r="B27" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="74"/>
+      <c r="B27" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="78"/>
       <c r="D27" s="39" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -8917,16 +8937,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B27:C27"/>
   </mergeCells>
   <conditionalFormatting sqref="D8:D13 D18:D19 D3:D6 D15:D16">
     <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
@@ -9145,7 +9165,7 @@
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B3" s="79" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C3" s="79"/>
       <c r="D3" s="79"/>
@@ -9153,7 +9173,7 @@
       <c r="F3" s="79"/>
       <c r="G3" s="79"/>
       <c r="I3" s="80" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J3" s="80"/>
       <c r="K3" s="80"/>
@@ -9161,22 +9181,22 @@
     </row>
     <row r="4" spans="2:12" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="40" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I4" s="80"/>
       <c r="J4" s="80"/>
@@ -9185,10 +9205,10 @@
     </row>
     <row r="5" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="81" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D5" s="44">
         <v>0</v>
@@ -9211,7 +9231,7 @@
     <row r="6" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="B6" s="81"/>
       <c r="C6" s="46" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D6" s="47">
         <v>0</v>
@@ -9228,7 +9248,7 @@
     <row r="7" spans="2:12" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="81"/>
       <c r="C7" s="46" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D7" s="47">
         <v>33</v>
@@ -9242,7 +9262,7 @@
       </c>
       <c r="G7" s="82"/>
       <c r="I7" s="83" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J7" s="83"/>
       <c r="K7" s="83"/>
@@ -9251,7 +9271,7 @@
     <row r="8" spans="2:12" s="1" customFormat="1">
       <c r="B8" s="81"/>
       <c r="C8" s="46" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D8" s="49">
         <v>0.2</v>
@@ -9272,7 +9292,7 @@
     <row r="9" spans="2:12" s="1" customFormat="1">
       <c r="B9" s="81"/>
       <c r="C9" s="46" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D9" s="49">
         <v>0.02</v>
@@ -9352,7 +9372,7 @@
     </row>
     <row r="15" spans="2:12" s="1" customFormat="1" ht="27.75" customHeight="1">
       <c r="B15" s="79" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="79"/>
@@ -9366,22 +9386,22 @@
     </row>
     <row r="16" spans="2:12" s="1" customFormat="1">
       <c r="B16" s="54" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F16" s="55" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I16" s="83"/>
       <c r="J16" s="83"/>
@@ -9390,10 +9410,10 @@
     </row>
     <row r="17" spans="2:12" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="B17" s="86" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D17" s="47">
         <v>0</v>
@@ -9416,7 +9436,7 @@
     <row r="18" spans="2:12" s="1" customFormat="1">
       <c r="B18" s="86"/>
       <c r="C18" s="57" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D18" s="58">
         <v>0</v>
@@ -9435,12 +9455,12 @@
       <c r="L18" s="83"/>
     </row>
     <row r="19" spans="2:12" s="1" customFormat="1">
-      <c r="B19" s="61"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="50"/>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
       <c r="F19" s="51"/>
-      <c r="G19" s="61"/>
+      <c r="G19" s="62"/>
     </row>
     <row r="20" spans="2:12" s="1" customFormat="1"/>
     <row r="21" spans="2:12" s="1" customFormat="1"/>
@@ -9591,10 +9611,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9605,29 +9625,29 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9635,7 +9655,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9643,20 +9663,20 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="C8" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="E9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>